<commit_message>
update: [API Loyalty] init.
</commit_message>
<xml_diff>
--- a/src/test/resources/init_data_excel/data_test_validation_customer.xlsx
+++ b/src/test/resources/init_data_excel/data_test_validation_customer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\back_ends\testing\app\src\test\resources\init_data_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA7185F-F552-478E-AEF9-66F2EA459FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84204522-87DB-4B96-957D-5F95816ECD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="1980" windowWidth="17280" windowHeight="8880" xr2:uid="{E4CAD842-3125-4AD6-9A96-475187D44F7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E4CAD842-3125-4AD6-9A96-475187D44F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="create" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Không được để trống email khách hàng.;Không đúng định dạng email khách hàng.</t>
+  </si>
+  <si>
+    <t>Thêm mới thành công.</t>
+  </si>
+  <si>
+    <t>Email [huytinhcd123@gmail.com] không hợp lệ.</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -517,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B1CEC1-3EB5-4B7C-B559-59FAD8DD7CED}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +537,7 @@
     <col min="3" max="3" width="39.88671875" customWidth="1"/>
     <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,28 +629,46 @@
       <c r="B4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="E4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{EEE12A01-3AA1-43D6-996B-881D85AE9E0F}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{6321BEDE-EC61-41E0-9593-DFB8CF5164F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>